<commit_message>
Updated paper notes and paper details
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885245B1-CD42-4ED8-A530-FA0EFFFB15DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6664218-1511-47D6-A27A-37763C156FC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Authors</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Monitoring and evaluation in conservation: a review of trends and approaches</t>
   </si>
   <si>
-    <t>Lack of data on past conservation investments</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -90,7 +87,58 @@
     <t>Changing spatial patterns of conservation investment by a major land trust</t>
   </si>
   <si>
-    <t>Investment of TNC over space and time</t>
+    <t>Although identifying priority regions is an important first step in solving this problem, it does not indicate how limited resources should be allocated between regions. Here we formulate how to allocate optimally conservation resources between regions identified as priorities for conservation—the ‘conservation resource allocation problem’. We identify two easy-to-use and easy-to-interpret heuristics that closely approximate the optimal solution. We also show the importance of both correctly formulating the problem and using information on how investment returns change through time.</t>
+  </si>
+  <si>
+    <t>Assessment of TNC's conservation investment between 1970-2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looked at conservation spending and land acquisition by the TNC between 1970 - 2009. They contrasted the area of land protected and upfront cost to TNC of protecting these areas as alternative measures of conservation effort. The results of our regression analyses are broadly consistent with an increasingly strategic signal to conservation investment patterns through time. </t>
+  </si>
+  <si>
+    <t>Assessing mgmgt effectiveness</t>
+  </si>
+  <si>
+    <t>Monitoring and evaluation of conservation projects</t>
+  </si>
+  <si>
+    <t>Mixed Effects of Long‐Term Conservation Investment in Natura 2000 Farmland</t>
+  </si>
+  <si>
+    <t>Santana et al</t>
+  </si>
+  <si>
+    <t>Provide a case study on the effectiveness of long-term conservation investment in N2000</t>
+  </si>
+  <si>
+    <t>Teshome</t>
+  </si>
+  <si>
+    <t>Tenure security and soil conservation investment decisions: Empirical evidence from East Gojam, Ethiopia</t>
+  </si>
+  <si>
+    <t>Modelled farmers willingness to invest in soil conservation</t>
+  </si>
+  <si>
+    <t>As expected, tenure insecurity has a significant negative influence on soil conservation investments. This suggests that tenure insecure households are less likely to invest in soil conservation technologies.</t>
+  </si>
+  <si>
+    <t>Lennox &amp; Armsworth</t>
+  </si>
+  <si>
+    <t>Suitability of short or long term conservation contracts under ecological and socio-economic uncertainty</t>
+  </si>
+  <si>
+    <t>In this paper, we examine the role that different kinds of uncertainty play in determining the relative advantages of short and long contracts. Specifically, we examine how uncertainty over future site availability and over future site ecological condition affects the choice of contract duration.</t>
+  </si>
+  <si>
+    <t>Modelling best strategies relating to short and long term conservation contracts</t>
+  </si>
+  <si>
+    <t>Murdoch et al</t>
+  </si>
+  <si>
+    <t>Using return on investment to maximise conservation effectiveness in Argentine grasslands</t>
   </si>
 </sst>
 </file>
@@ -107,13 +155,14 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF1C1D1E"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
+      <color rgb="FF1C1D1E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,15 +188,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,17 +514,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="82.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -487,149 +539,196 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2007</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2006</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2006</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C6" s="2">
         <v>2003</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C7" s="2">
         <v>2005</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2013</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2011</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated paper details, notes, and powerpoint
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA055594-109F-436A-AB40-145B604BF974}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7803885-523B-4360-97C3-8CE7E0A8D601}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Authors</t>
   </si>
@@ -157,6 +157,96 @@
   </si>
   <si>
     <t>Modelled people's willingness to invest in conservation-focused livelihoods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our study showed mixed effects of long-term conservation investment in N2000 farmland. We found positive effects on flagship species, and on species associated with fallows, which were the main targets of conservation investment. Finally, long-term evaluations of conservation investment are required, in order to monitor and improve the effectiveness of billions of euros needed annually for managing N2000. </t>
+  </si>
+  <si>
+    <t>Fryxell et al</t>
+  </si>
+  <si>
+    <t>Resource management cycles and the sustainability of harvested wildlife populations</t>
+  </si>
+  <si>
+    <t>Modelled complex dynamic relatinoships between harvest quotas, users, managers, and population survival</t>
+  </si>
+  <si>
+    <t>Here we show that weak compensatory response by harvesters or resource managers can itself generate cyclic variation in resources, exacerbating the risk of collapse. Weak harvest regulation contributes to the problem rather than providing an acceptable management solution to resource fluctuation. Our simulations suggest that the risk of population collapse could be dramatically higher in systems with dynamic effort and quota levels (Fig. 3), simply because of extreme population excursions caused by quasiperiodic dynamics resulting from even mild levels of environmental stochasticity.</t>
+  </si>
+  <si>
+    <t>Armsworth et al</t>
+  </si>
+  <si>
+    <t>Is conservation right to go big? PA size and conservation return on invesment</t>
+  </si>
+  <si>
+    <t>Examine how PA size influences conservation return on investment</t>
+  </si>
+  <si>
+    <t>Policy guidelines for creating new protected areas commonly recommend larger protected areas be favored. We examine whether these recommendations are justified, providing the first evaluation of this question to use return-on-investment (ROI) methods that account for how protected area size influences multiple ecological benefits and the economic costs of protection. A portfolio of site sizes may need to be included in protected area networks when multiple objectives motivate conservation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lindsey et al </t>
+  </si>
+  <si>
+    <t>Underperformance of African PA networks and the case for new conservation models: Insights from Zambia</t>
+  </si>
+  <si>
+    <t>Assess why PAs in Zambia are not performing well</t>
+  </si>
+  <si>
+    <t>They mention increasing human population increases in and around PAs is having a negative effect</t>
+  </si>
+  <si>
+    <t>Wittemyer et al</t>
+  </si>
+  <si>
+    <t>Accelerated human population growth at protected area edges</t>
+  </si>
+  <si>
+    <t>Assess human pop growth around PAs in 45 countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrary to predictions of this argument, we found that average human population growth rates on the borders of 306 PAs in 45 countries in Africa and Latin America were nearly double average rural growth, suggesting that PAs attract, rather than repel, human settlement. Human growth rate around PAs correlated with forest loss. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruner et al </t>
+  </si>
+  <si>
+    <t>Financial costs and shortfalls for expanding PA systems in developing countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference for the efficent use of PA resources and investment </t>
+  </si>
+  <si>
+    <t>Utami et al</t>
+  </si>
+  <si>
+    <t>Prioritizing management strategies to achieve multiple outcomes in a globally significant Indonesian protected area</t>
+  </si>
+  <si>
+    <t>Assessed different mgmt strategies for cost effectiveness and ability to improve a number of PA values over 15 years</t>
+  </si>
+  <si>
+    <t>in this study we aimed to: (a) build an approach capable of assessing the cost, relative bene- fits and cost-effectiveness of implementing threat management strategies that improve a broad range of values in multifunctional areas; (b) bring together and build key information to help managers and stakeholders understand the values, goals, threats, total management costs and opportunities for achieving goals for values, using the TNBB as a case study; and (c) deliver a set of costed, prioritized strategies for achieving goals across multiple important values of the TNBB.</t>
+  </si>
+  <si>
+    <t>Cullen</t>
+  </si>
+  <si>
+    <t>Biodiversity protection prioiritisation: a 25 year review</t>
+  </si>
+  <si>
+    <t>Meir et al</t>
+  </si>
+  <si>
+    <t>Does conservation planning matter in a dynamic and uncertain world?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here we explicitly consider the implications for biodiversity conservation of several key assumptions underlying systematic conservation planning methods. Our results suggest that relatively simple rules for deciding which areas to protect outperform both ad hoc investment strategies and comprehensive conservation plans (Figs 1 and 2). This is especially true when degradation rates and uncertainty are high </t>
+  </si>
+  <si>
+    <t>Simulate site selection under conditions of different budgets, site acquisition uncertainty</t>
   </si>
 </sst>
 </file>
@@ -532,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,7 +717,9 @@
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -727,40 +819,133 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+    <row r="12" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2010</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2008</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2004</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2004</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated paper notes and details
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7803885-523B-4360-97C3-8CE7E0A8D601}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720B6FD4-4CA9-4663-B595-41589353945E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>Authors</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Assessed different mgmt strategies for cost effectiveness and ability to improve a number of PA values over 15 years</t>
   </si>
   <si>
-    <t>in this study we aimed to: (a) build an approach capable of assessing the cost, relative bene- fits and cost-effectiveness of implementing threat management strategies that improve a broad range of values in multifunctional areas; (b) bring together and build key information to help managers and stakeholders understand the values, goals, threats, total management costs and opportunities for achieving goals for values, using the TNBB as a case study; and (c) deliver a set of costed, prioritized strategies for achieving goals across multiple important values of the TNBB.</t>
-  </si>
-  <si>
     <t>Cullen</t>
   </si>
   <si>
@@ -247,6 +244,87 @@
   </si>
   <si>
     <t>Simulate site selection under conditions of different budgets, site acquisition uncertainty</t>
+  </si>
+  <si>
+    <t>Reviews SCP literature</t>
+  </si>
+  <si>
+    <t>in this study we aimed to: (a) build an approach capable of assessing the cost, relative benefits and cost-effectiveness of implementing threat management strategies that improve a broad range of values in multifunctional areas; (b) bring together and build key information to help managers and stakeholders understand the values, goals, threats, total management costs and opportunities for achieving goals for values, using the TNBB as a case study; and (c) deliver a set of costed, prioritized strategies for achieving goals across multiple important values of the TNBB.</t>
+  </si>
+  <si>
+    <t>Vivitskaia et al</t>
+  </si>
+  <si>
+    <t>Linking threat maps with management to guide conservation investment</t>
+  </si>
+  <si>
+    <t>Built impact maps for coastal waters around the world and identified best strategies for investement for top 10 places</t>
+  </si>
+  <si>
+    <t>We rebuild cumulative impact maps by stressor type (climate change, marine and land) at a global scale to evaluate the expected effectiveness of various management strategies for all coastal territories. Key disparities were found between broad-scale management of marine ecosystems and the dominant stressors, with existing management in tropical island nations likely insufficient to address intense impacts from climate change. These countries also typically had low performance on governance indicators, suggesting challenges in implementing new mitigation. We highlight trade-offs in making decisions for stressor mitigation and offer strategic guidance on identifying locations to target management of marine, land, or climate impacts.</t>
+  </si>
+  <si>
+    <t>Our asset framework offers a complementary investment approach and proposition. The world is awash with capital but typical returns on investments are historically low. This, in combination with ideas of impact investing, is generating a demand for conservation investment products. Once formalised, a PA asset approach would create the capacity to optimize PA assets (as sites or networks) in terms of their spatial location, investment profile, and the forms of value they generate over time. It would also support and extend the programme of work on PA management effectiveness (Coad et al., 2015) through providing a framework to assess the social, economic and cultural benefits of PAs.</t>
+  </si>
+  <si>
+    <t>Argue for framing PAs as spatial assets for generating investment</t>
+  </si>
+  <si>
+    <t>Jepson et al</t>
+  </si>
+  <si>
+    <t>Protected area asset stewardship</t>
+  </si>
+  <si>
+    <t>Kearney et al</t>
+  </si>
+  <si>
+    <t>Estimating the benefit of well-managed protected areas for threatened speices conservation</t>
+  </si>
+  <si>
+    <t>Use Australia PA network as example of under-resourced PAs not protecting species</t>
+  </si>
+  <si>
+    <t>Good reference for the case for adequately investing in protected areas. Also warn against expanding PA networks without ensureing adequte resources for those PAs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coad et al </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widespread shortfalls in protected area resourcing undermine efforts to conserve biodiversity </t>
+  </si>
+  <si>
+    <t>assess &gt;2100 PA reports and quantify how many are under funded and resourced</t>
+  </si>
+  <si>
+    <t>Pringle</t>
+  </si>
+  <si>
+    <t>Upgrading protected areas to conserve wild biodiversity</t>
+  </si>
+  <si>
+    <t>Uses two case studies to show how PAs can be expanded and rewilded</t>
+  </si>
+  <si>
+    <t>International agreements mandate the expansion of Earth's protected-area network as a bulwark against the continued extinction of wild populations, species, and ecosystems. Yet many protected areas are underfunded, poorly managed, and ecologically damaged; the conundrum is how to increase their coverage and effectiveness simultaneously. Worldwide, enormous potential for biodiversity conservation can be realized by upgrading existing nature reserves while harmonizing them with the needs and aspirations of their constituencies.</t>
+  </si>
+  <si>
+    <t>Robinson et al</t>
+  </si>
+  <si>
+    <t>Incorporating land tenure security into conservation</t>
+  </si>
+  <si>
+    <t>present a framework that identifies three common ways in which land tenure security can impact human and conservation outcomes</t>
+  </si>
+  <si>
+    <t>Insecure land tenure plagues many developing and tropical regions, often where conservation concerns are highest. We present a framework that identifies three common ways in which land tenure security can impact human and conservation outcomes, and suggest practical ways to distill tenure and tenure security issues for a given location. We conclude with steps for considering tenure security issues in the context of conservation projects and identify areas for future research.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de Oliveira et al </t>
+  </si>
+  <si>
+    <t>The financial needs vs. the realities of in situ conservation: an analysis of federal funding for protected areas in Brazil's Caatinga</t>
   </si>
 </sst>
 </file>
@@ -622,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,35 +994,148 @@
         <v>63</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C18" s="2">
         <v>2012</v>
       </c>
+      <c r="D18" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C19" s="2">
         <v>2004</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated investment powerpoint & paper details Excel
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720B6FD4-4CA9-4663-B595-41589353945E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640BED0D-C1C0-4014-AAF7-1B26F7308F20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
@@ -702,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Paper details - minor edits
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1456F29C-C26C-482E-9ECC-DF5DEAB92D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D315E240-0E2C-4125-8585-E2D9F502B51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated papers and paper details excel
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D315E240-0E2C-4125-8585-E2D9F502B51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B75842-F3DA-4A41-8418-7584738A4F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>Authors</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Incorporating the effects of socioeconomic uncertainty into priority setting for conservation investment</t>
   </si>
   <si>
-    <t>Uncertainty in the implementation and outcomes of conservation actions that is not accounted for leaves conservation plans vulnerable to potential changes in future conditions. We used a decision‐theoretic approach to investigate the effects of two types of investment uncertainty on the optimal allocation of global conservation resources for land acquisition in the Mediterranean Basin. We considered uncertainty about (1) whether investment will continue and (2) whether the acquired biodiversity assets are secure, which we termed transaction uncertainty and performance uncertainty, respectively.  In the presence of uncertainty in future investment ability (transaction uncertainty), the optimal strategy was opportunistic, meaning the investment priority should be to act where uncertainty is highest while investment remains possible. The improved performance of rules of thumb when accounting for uncertainty highlights the importance of explicitly incorporating sources of investment uncertainty and evaluating potential conservation investments in the context of their likely long‐term success.</t>
-  </si>
-  <si>
     <t>Prioritising global conservation efforts</t>
   </si>
   <si>
@@ -87,15 +84,9 @@
     <t>Changing spatial patterns of conservation investment by a major land trust</t>
   </si>
   <si>
-    <t>Although identifying priority regions is an important first step in solving this problem, it does not indicate how limited resources should be allocated between regions. Here we formulate how to allocate optimally conservation resources between regions identified as priorities for conservation—the ‘conservation resource allocation problem’. We identify two easy-to-use and easy-to-interpret heuristics that closely approximate the optimal solution. We also show the importance of both correctly formulating the problem and using information on how investment returns change through time.</t>
-  </si>
-  <si>
     <t>Assessment of TNC's conservation investment between 1970-2009</t>
   </si>
   <si>
-    <t xml:space="preserve">Looked at conservation spending and land acquisition by the TNC between 1970 - 2009. They contrasted the area of land protected and upfront cost to TNC of protecting these areas as alternative measures of conservation effort. The results of our regression analyses are broadly consistent with an increasingly strategic signal to conservation investment patterns through time. </t>
-  </si>
-  <si>
     <t>Assessing mgmgt effectiveness</t>
   </si>
   <si>
@@ -120,18 +111,12 @@
     <t>Modelled farmers willingness to invest in soil conservation</t>
   </si>
   <si>
-    <t>As expected, tenure insecurity has a significant negative influence on soil conservation investments. This suggests that tenure insecure households are less likely to invest in soil conservation technologies.</t>
-  </si>
-  <si>
     <t>Lennox &amp; Armsworth</t>
   </si>
   <si>
     <t>Suitability of short or long term conservation contracts under ecological and socio-economic uncertainty</t>
   </si>
   <si>
-    <t>In this paper, we examine the role that different kinds of uncertainty play in determining the relative advantages of short and long contracts. Specifically, we examine how uncertainty over future site availability and over future site ecological condition affects the choice of contract duration.</t>
-  </si>
-  <si>
     <t>Modelling best strategies relating to short and long term conservation contracts</t>
   </si>
   <si>
@@ -144,24 +129,15 @@
     <t xml:space="preserve">Modelling best strategies for conserving Argentine grasslands </t>
   </si>
   <si>
-    <t>Modelled three different strategies for selecting 10% of a huge area of Argentine grasslands. Minimise cost, maximise gain, and then return on investment. The ROI strategy was by far the best. The maximise gain was by far the worst as the costs were extremely high</t>
-  </si>
-  <si>
     <t>Jansen et al</t>
   </si>
   <si>
     <t>Determinants of income-earning strategies and adoption of conservation practices in hillside communities in rural Honduras</t>
   </si>
   <si>
-    <t>State that population increases and insecure tenure have caused forest loss. The results regarding the influence of population density on conservation practices suggest a U-type relationship. That is, up to a certain population density the four conservation practices considered here are less common in communities with higher population densities. However, after a certain point population density has a positive influence on the adoption of conservation practices.</t>
-  </si>
-  <si>
     <t>Modelled people's willingness to invest in conservation-focused livelihoods</t>
   </si>
   <si>
-    <t xml:space="preserve">Our study showed mixed effects of long-term conservation investment in N2000 farmland. We found positive effects on flagship species, and on species associated with fallows, which were the main targets of conservation investment. Finally, long-term evaluations of conservation investment are required, in order to monitor and improve the effectiveness of billions of euros needed annually for managing N2000. </t>
-  </si>
-  <si>
     <t>Fryxell et al</t>
   </si>
   <si>
@@ -171,9 +147,6 @@
     <t>Modelled complex dynamic relatinoships between harvest quotas, users, managers, and population survival</t>
   </si>
   <si>
-    <t>Here we show that weak compensatory response by harvesters or resource managers can itself generate cyclic variation in resources, exacerbating the risk of collapse. Weak harvest regulation contributes to the problem rather than providing an acceptable management solution to resource fluctuation. Our simulations suggest that the risk of population collapse could be dramatically higher in systems with dynamic effort and quota levels (Fig. 3), simply because of extreme population excursions caused by quasiperiodic dynamics resulting from even mild levels of environmental stochasticity.</t>
-  </si>
-  <si>
     <t>Armsworth et al</t>
   </si>
   <si>
@@ -207,9 +180,6 @@
     <t>Assess human pop growth around PAs in 45 countries</t>
   </si>
   <si>
-    <t xml:space="preserve">Contrary to predictions of this argument, we found that average human population growth rates on the borders of 306 PAs in 45 countries in Africa and Latin America were nearly double average rural growth, suggesting that PAs attract, rather than repel, human settlement. Human growth rate around PAs correlated with forest loss. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bruner et al </t>
   </si>
   <si>
@@ -240,18 +210,12 @@
     <t>Does conservation planning matter in a dynamic and uncertain world?</t>
   </si>
   <si>
-    <t xml:space="preserve">Here we explicitly consider the implications for biodiversity conservation of several key assumptions underlying systematic conservation planning methods. Our results suggest that relatively simple rules for deciding which areas to protect outperform both ad hoc investment strategies and comprehensive conservation plans (Figs 1 and 2). This is especially true when degradation rates and uncertainty are high </t>
-  </si>
-  <si>
     <t>Simulate site selection under conditions of different budgets, site acquisition uncertainty</t>
   </si>
   <si>
     <t>Reviews SCP literature</t>
   </si>
   <si>
-    <t>in this study we aimed to: (a) build an approach capable of assessing the cost, relative benefits and cost-effectiveness of implementing threat management strategies that improve a broad range of values in multifunctional areas; (b) bring together and build key information to help managers and stakeholders understand the values, goals, threats, total management costs and opportunities for achieving goals for values, using the TNBB as a case study; and (c) deliver a set of costed, prioritized strategies for achieving goals across multiple important values of the TNBB.</t>
-  </si>
-  <si>
     <t>Vivitskaia et al</t>
   </si>
   <si>
@@ -261,12 +225,6 @@
     <t>Built impact maps for coastal waters around the world and identified best strategies for investement for top 10 places</t>
   </si>
   <si>
-    <t>We rebuild cumulative impact maps by stressor type (climate change, marine and land) at a global scale to evaluate the expected effectiveness of various management strategies for all coastal territories. Key disparities were found between broad-scale management of marine ecosystems and the dominant stressors, with existing management in tropical island nations likely insufficient to address intense impacts from climate change. These countries also typically had low performance on governance indicators, suggesting challenges in implementing new mitigation. We highlight trade-offs in making decisions for stressor mitigation and offer strategic guidance on identifying locations to target management of marine, land, or climate impacts.</t>
-  </si>
-  <si>
-    <t>Our asset framework offers a complementary investment approach and proposition. The world is awash with capital but typical returns on investments are historically low. This, in combination with ideas of impact investing, is generating a demand for conservation investment products. Once formalised, a PA asset approach would create the capacity to optimize PA assets (as sites or networks) in terms of their spatial location, investment profile, and the forms of value they generate over time. It would also support and extend the programme of work on PA management effectiveness (Coad et al., 2015) through providing a framework to assess the social, economic and cultural benefits of PAs.</t>
-  </si>
-  <si>
     <t>Argue for framing PAs as spatial assets for generating investment</t>
   </si>
   <si>
@@ -285,9 +243,6 @@
     <t>Use Australia PA network as example of under-resourced PAs not protecting species</t>
   </si>
   <si>
-    <t>Good reference for the case for adequately investing in protected areas. Also warn against expanding PA networks without ensureing adequte resources for those PAs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coad et al </t>
   </si>
   <si>
@@ -306,9 +261,6 @@
     <t>Uses two case studies to show how PAs can be expanded and rewilded</t>
   </si>
   <si>
-    <t>International agreements mandate the expansion of Earth's protected-area network as a bulwark against the continued extinction of wild populations, species, and ecosystems. Yet many protected areas are underfunded, poorly managed, and ecologically damaged; the conundrum is how to increase their coverage and effectiveness simultaneously. Worldwide, enormous potential for biodiversity conservation can be realized by upgrading existing nature reserves while harmonizing them with the needs and aspirations of their constituencies.</t>
-  </si>
-  <si>
     <t>Robinson et al</t>
   </si>
   <si>
@@ -325,13 +277,480 @@
   </si>
   <si>
     <t>The financial needs vs. the realities of in situ conservation: an analysis of federal funding for protected areas in Brazil's Caatinga</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uncertainty in the implementation and outcomes of conservation action</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s that is not accounted for leaves conservation plans vulnerable to potential changes in future conditions. We used a decision‐theoretic approach to investigate the effects of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> two types of investment uncertainty on the optimal allocation of global conservation resources for land acquisition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the Mediterranean Basin. We considered uncertainty about (1) whether investment will continue and (2) whether the acquired biodiversity assets are secure, which we termed transaction uncertainty and performance uncertainty, respectively.  In the presence of uncertainty in future investment ability (transaction uncertainty), the optimal strategy was opportunistic, meaning the investment priority should be to act where uncertainty is highest while investment remains possible. The improved performance of rules of thumb when accounting for uncertainty highlights the importance of explicitly incorporating sources of investment uncertainty and evaluating potential conservation investments in the context of their likely long‐term success.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Although identifying priority regions is an important first step in solving this problem, it does not indicate how limited resources should be allocated between regions. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Here we formulate how to allocate optimally conservation resources between regions identified as priorities for conservation—the ‘conservation resource allocation problem’</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. We identify two easy-to-use and easy-to-interpret heuristics that closely approximate the optimal solution. We also show the importance of both correctly formulating the problem and using information on how investment returns change through time.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Looked at conservation spending and land acquisition by the TNC between 1970 - 2009. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">They contrasted the area of land protected and upfront cost to TNC of protecting these areas as alternative measures of conservation effort. The results of our regression analyses </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>are broadly consistent with an increasingly strategic signal to conservation investment patterns through time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Our study showed mixed effects of long-term conservation investment in N2000 farmland</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. We found positive effects on flagship species, and on species associated with fallows, which were the main targets of conservation investment. Finally, long-term evaluations of conservation investment are required, in order to monitor and improve the effectiveness of billions of euros needed annually for managing N2000. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System wide PA management effectivess assessments can enable policymakers to refine their conservation strategies, reallocate budget expenditures, and develop strategic, systemwide responses to the most pervasive threats and management weaknesses. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inadequate funding was a serious weakness for all the countries studied except Bhutan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. funding was not considered adequate to conduct critical management activities, defined as any management activities that prevent irreplaceable or unacceptable losses to natural or cultural resources. Inadequate
+funding has led directly to a raft of other management problems, including inadequate field equipment, transportation, and facilities. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Underfunding of protected areas appears to be a systemic problem in other areas of the world;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">As expected, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tenure insecurity has a significant negative influence on soil conservation investments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. This suggests that tenure insecure households are less likely to invest in soil conservation technologies.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In this paper, we examine the role that different kinds of uncertainty play in determining the relative advantages of short and long contracts. Specifically, we examine how uncertainty over future site availability and over future site ecological condition affects the choice of contract duration. we investigate how </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the choice between short or long conservation contracts is affected by uncertainty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> regarding the future availability of sites and their ecological condition.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modelled three different strategies for selecting 10% of a huge area of Argentine grasslands</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Minimise cost, maximise gain, and then return on investment. The ROI strategy was by far the best. The maximise gain was by far the worst as the costs were extremely high</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>State that population increases and insecure tenure have caused forest loss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. The results regarding the influence of population density on conservation practices suggest a U-type relationship. That is, up to a certain population density the four conservation practices considered here are less common in communities with higher population densities. However, after a certain point population density has a positive influence on the adoption of conservation practices.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Here we show that weak compensatory response by harvesters or resource managers can itself generate cyclic variation in resources, exacerbating the risk of collapse. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weak harvest regulation contributes to the problem rather than providing an acceptable management solution to resource fluctuation. Our simulations suggest that the risk of population collapse could be dramatically higher in systems with dynamic effort and quota levels (Fig. 3),</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> simply because of extreme population excursions caused by quasiperiodic dynamics resulting from even mild levels of environmental stochasticity.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Contrary to predictions of this argument, we found that average human population growth rates on the borders of 306 PAs in 45 countries in Africa and Latin America were nearly double average rural growth, suggesting </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>that PAs attract, rather than repel, human settlement. Human growth rate around PAs correlated with forest loss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in this study we aimed to: (a) build an approach capable of assessing the cost, relative benefits and cost-effectiveness of implementing threat management strategies that improve a broad range of values in multifunctional areas; (b) bring together and build key information to help managers and stakeholders understand the values, goals, threats, total management costs and opportunities for achieving goals for values, using the TNBB as a case study; and (c) deliver a set of costed, prioritized strategies for achieving goals across multiple important values of the TNBB. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quantified the required investment to improve all areas of PA, followed by the most cost effective strategies (i.e., if you has less, whats the best investment)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Here we explicitly consider the implications for biodiversity conservation of several key assumptions underlying systematic conservation planning methods. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Our results suggest that relatively simple rules for deciding which areas to protect outperform both ad hoc investment strategies and comprehensive conservation plans </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Figs 1 and 2). This is especially true when degradation rates and uncertainty are high </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>We rebuild cumulative impact maps by stressor type (climate change, marine and land) at a global scale to evaluate the expected effectiveness of various management strategies for all coastal territories</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Key disparities were found between broad-scale management of marine ecosystems and the dominant stressors, with existing management in tropical island nations likely insufficient to address intense impacts from climate change. These countries also typically had low performance on governance indicators, suggesting challenges in implementing new mitigation. We highlight trade-offs in making decisions for stressor mitigation and offer strategic guidance on identifying locations to target management of marine, land, or climate impacts.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Our asset framework offers a complementary investment approach and proposition. The world is awash with capital but typical returns on investments are historically low. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This, in combination with ideas of impact investing, is generating a demand for conservation investment products. Once formalised, a PA asset approach would create the capacity to optimize PA assets (as sites or networks) in terms of their spatial location, investment profile, and the forms of value they generate over time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. It would also support and extend the programme of work on PA management effectiveness (Coad et al., 2015) through providing a framework to assess the social, economic and cultural benefits of PAs.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Good reference for the case for adequately investing in protected areas. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Also warn against expanding PA networks without ensureing adequte resources for those PAs</t>
+    </r>
+  </si>
+  <si>
+    <t>Assess 2167 PA management reports, and less than a quarter report having sufficient resources in terms of budget and staffing</t>
+  </si>
+  <si>
+    <r>
+      <t>International agreements mandate the expansion of Earth's protected-area network as a bulwark against the continued extinction of wild populations, species, and ecosystems.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Yet many protected areas are underfunded, poorly managed, and ecologically damaged</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; the conundrum is how to increase their coverage and effectiveness simultaneously. Worldwide, enormous potential for biodiversity conservation can be realized by upgrading existing nature reserves while harmonizing them with the needs and aspirations of their constituencies.</t>
+    </r>
+  </si>
+  <si>
+    <t>Looked at finances in subset of Braziliian PA - uneven funding, all underfunded</t>
+  </si>
+  <si>
+    <r>
+      <t>we analyzed the Brazilian Government’s budget allocated to 20 federal PAs in the Caatinga
+between 2008 and 2014, which ranged from 231,575 USD in 2008 to 13.5 Mi USD in 2011. Land acquisition in a single PA consumed ~75% of the budget, and the two smallest PAs received proportionally the most money. Excluding land acquisition, the 20 PAs received 0.50 USD/ha/year.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Funds were allocated not to biodiversity conservation per se but mainly to securing offices, cars, and equipment. Even including salaries, the budget allocated for these PAs is ~13 times lower than what the Ministry of the Environment declared necessary for the basic operation of protected areas in Brazil</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +768,13 @@
     <font>
       <sz val="9"/>
       <color rgb="FF1C1D1E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -374,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,6 +811,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -744,400 +1174,411 @@
         <v>2007</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>2006</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="2">
         <v>2013</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <v>2013</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>2003</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>2005</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2">
         <v>2014</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2">
         <v>2011</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2">
         <v>2010</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2">
         <v>2006</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2">
         <v>2010</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2">
         <v>2018</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2">
         <v>2014</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2">
         <v>2008</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2">
         <v>2004</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2">
         <v>2020</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2">
         <v>2012</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2">
         <v>2004</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2">
         <v>2020</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2">
         <v>2017</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C22" s="2">
         <v>2018</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2">
         <v>2019</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2">
         <v>2017</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2">
         <v>2017</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2">
         <v>2017</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Highlighting important text in Excel paper spreadsheet
</commit_message>
<xml_diff>
--- a/Papers/Paper_details.xlsx
+++ b/Papers/Paper_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B75842-F3DA-4A41-8418-7584738A4F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2893CA-F5E5-4B29-9884-2BC4A17C0A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99DDE1EE-4B93-4F2F-A8F6-CFC06F5CA5F4}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>Reviews SCP literature</t>
   </si>
   <si>
-    <t>Vivitskaia et al</t>
-  </si>
-  <si>
     <t>Linking threat maps with management to guide conservation investment</t>
   </si>
   <si>
@@ -744,6 +741,9 @@
       </rPr>
       <t xml:space="preserve"> Funds were allocated not to biodiversity conservation per se but mainly to securing offices, cars, and equipment. Even including salaries, the budget allocated for these PAs is ~13 times lower than what the Ministry of the Environment declared necessary for the basic operation of protected areas in Brazil</t>
     </r>
+  </si>
+  <si>
+    <t>Tulloch et al</t>
   </si>
 </sst>
 </file>
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38B344F-7026-4A46-8EA5-561F1CA41D05}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
@@ -1194,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
@@ -1211,7 +1211,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
@@ -1228,7 +1228,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
@@ -1245,7 +1245,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
@@ -1277,7 +1277,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
@@ -1294,7 +1294,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
@@ -1311,7 +1311,7 @@
         <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
         <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
@@ -1345,7 +1345,7 @@
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
@@ -1396,7 +1396,7 @@
         <v>47</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
@@ -1428,7 +1428,7 @@
         <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
@@ -1459,126 +1459,126 @@
         <v>58</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C20" s="2">
         <v>2020</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C21" s="2">
         <v>2017</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C22" s="2">
         <v>2018</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C23" s="2">
         <v>2019</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="60.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C24" s="2">
         <v>2017</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C25" s="2">
         <v>2017</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="84.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C26" s="2">
         <v>2017</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>